<commit_message>
Added model selection routine for survey and site variables
</commit_message>
<xml_diff>
--- a/data/pointCount/TTA5-1_ISS_20171003.xlsx
+++ b/data/pointCount/TTA5-1_ISS_20171003.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/Team Drives/Biodiversity/CAGN occupancy/Point counts/2017/Landak October/Point Counts/toBeProofed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathe\Documents\songbird-occupancy\data\pointCount\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854DA669-5847-4FE1-BF19-EF8401ABB47A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7620" tabRatio="500"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
   <definedNames>
     <definedName name="species">'Species list'!$A$2:$A$444</definedName>
   </definedNames>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="130407"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="422">
   <si>
     <t>Geopelia striata</t>
   </si>
@@ -1316,9 +1317,6 @@
   </si>
   <si>
     <t>IMG_20171006_161927.jpg</t>
-  </si>
-  <si>
-    <t>Arachnothera Longirostra</t>
   </si>
   <si>
     <t>Cannot hear</t>
@@ -1333,7 +1331,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1721,25 +1719,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="4" width="11" style="2"/>
     <col min="5" max="5" width="11" style="1"/>
-    <col min="6" max="6" width="15.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.80859375" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="3"/>
     <col min="8" max="9" width="11" style="2"/>
-    <col min="10" max="10" width="15.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" style="2" customWidth="1"/>
     <col min="11" max="11" width="24.6640625" style="2" customWidth="1"/>
     <col min="12" max="12" width="23.6640625" style="2" customWidth="1"/>
     <col min="13" max="13" width="11" style="2"/>
-    <col min="14" max="14" width="30.1640625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="30.140625" style="6" customWidth="1"/>
     <col min="15" max="15" width="11" style="2"/>
     <col min="16" max="16" width="11" style="3"/>
     <col min="18" max="18" width="11" style="3"/>
@@ -1747,7 +1745,7 @@
     <col min="20" max="22" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>200</v>
       </c>
@@ -1815,7 +1813,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>410</v>
       </c>
@@ -1850,7 +1848,7 @@
         <v>418</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>411</v>
@@ -1877,7 +1875,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>410</v>
       </c>
@@ -1912,13 +1910,13 @@
         <v>418</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>411</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>419</v>
+        <v>62</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>414</v>
@@ -1939,7 +1937,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>410</v>
       </c>
@@ -1974,7 +1972,7 @@
         <v>418</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>411</v>
@@ -2001,7 +1999,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>410</v>
       </c>
@@ -2036,7 +2034,7 @@
         <v>418</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>411</v>
@@ -2063,7 +2061,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>410</v>
       </c>
@@ -2098,13 +2096,13 @@
         <v>418</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>411</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>414</v>
@@ -2122,13 +2120,13 @@
         <v>1.1574074074074073E-3</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="U6" s="4" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>410</v>
       </c>
@@ -2163,7 +2161,7 @@
         <v>418</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>411</v>
@@ -2190,7 +2188,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>410</v>
       </c>
@@ -2225,13 +2223,13 @@
         <v>418</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>411</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>414</v>
@@ -2249,13 +2247,13 @@
         <v>3.0671296296296297E-3</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="U8" s="4" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>410</v>
       </c>
@@ -2290,7 +2288,7 @@
         <v>418</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>411</v>
@@ -2317,7 +2315,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>410</v>
       </c>
@@ -2352,7 +2350,7 @@
         <v>418</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>411</v>
@@ -2379,7 +2377,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -2390,7 +2388,7 @@
       <c r="O11" s="4"/>
       <c r="U11" s="4"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -2401,7 +2399,7 @@
       <c r="O12" s="4"/>
       <c r="U12" s="4"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -2412,7 +2410,7 @@
       <c r="O13" s="4"/>
       <c r="U13" s="4"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -2423,7 +2421,7 @@
       <c r="O14" s="4"/>
       <c r="U14" s="4"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.4">
       <c r="B15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -2434,91 +2432,91 @@
       <c r="O15" s="4"/>
       <c r="U15" s="4"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.4">
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations xWindow="601" yWindow="221" count="20">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" error="Please choose one option from the drop down list." promptTitle="Lokasi survey" prompt="Tulis nama lokasi survey. Pilih satu dari daftarnya." sqref="A1:A1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" error="Please choose one option from the drop down list." promptTitle="Lokasi survey" prompt="Tulis nama lokasi survey. Pilih satu dari daftarnya." sqref="A1:A1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Dawar, Umbo, Semadum, Tauk"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" promptTitle="Pengawas primer" prompt="Tulis nama orang yang menulis data sheet ini." sqref="C2:C1048576">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" promptTitle="Pengawas primer" prompt="Tulis nama orang yang menulis data sheet ini." sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>3</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" promptTitle="Nama pengawas kedua" prompt="Tulis nama pasangan pengawas pertama." sqref="D1:D1048576">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" promptTitle="Nama pengawas kedua" prompt="Tulis nama pasangan pengawas pertama." sqref="D1:D1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>3</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" error="Please enter the name of the point" promptTitle="No. Titik" prompt="Tulis nomor titik ini." sqref="B1:B1048576">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" error="Please enter the name of the point" promptTitle="No. Titik" prompt="Tulis nomor titik ini." sqref="B1:B1048576" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>2</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
+    <dataValidation type="date" operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>40543</formula1>
     </dataValidation>
-    <dataValidation type="time" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Jam mulai" prompt="Tulis jam mulai saja. Tidak usah menulis jam berhenti." sqref="F1:F1048576">
+    <dataValidation type="time" operator="greaterThan" showInputMessage="1" showErrorMessage="1" promptTitle="Jam mulai" prompt="Tulis jam mulai saja. Tidak usah menulis jam berhenti." sqref="F1:F1048576" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0.166666666666667</formula1>
     </dataValidation>
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" promptTitle="Pengawas pertama" prompt="Tulis nama orang yang menulis data sheet ini." sqref="C1">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" promptTitle="Pengawas pertama" prompt="Tulis nama orang yang menulis data sheet ini." sqref="C1" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>3</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" sqref="H1:J1048576">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" sqref="H1:J1048576" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="O2:O1048576" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"A, V, F"</formula1>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="P1:P1048576">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="P1:P1048576" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="Pilih satu dari dafter. 0 berarti jumlah utk spesis ini tidak merupakan perkiraan. 1 berarti jumlah utk spesis ini merupakan perkiraan." sqref="Q1:Q1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="Pilih satu dari dafter. 0 berarti jumlah utk spesis ini tidak merupakan perkiraan. 1 berarti jumlah utk spesis ini merupakan perkiraan." sqref="Q1:Q1048576" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"0,1"</formula1>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" prompt="0 = tidak diketahui_x000d_1 = 0-25m_x000d_2 = 25-50m_x000d_3 = 50-75m_x000d_4 = 75-100m" sqref="R1:R1048576">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" prompt="0 = tidak diketahui_x000d_1 = 0-25m_x000d_2 = 25-50m_x000d_3 = 50-75m_x000d_4 = 75-100m" sqref="R1:R1048576" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>0</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="time" showInputMessage="1" showErrorMessage="1" prompt="Tulis waktu rekaman. Waktu ini berupa minit sama detik dari detik mulai point count, bukan waktu dari awal rekaman." sqref="S1:S1048576">
+    <dataValidation type="time" showInputMessage="1" showErrorMessage="1" prompt="Tulis waktu rekaman. Waktu ini berupa minit sama detik dari detik mulai point count, bukan waktu dari awal rekaman." sqref="S1:S1048576" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>0</formula1>
       <formula2>0.416666666666667</formula2>
     </dataValidation>
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" prompt="Tulis nama orang yg memasukkan data ke data sheet ini. Seharusnya kamu!" sqref="U1:U1048576">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" prompt="Tulis nama orang yg memasukkan data ke data sheet ini. Seharusnya kamu!" sqref="U1:U1048576" xr:uid="{00000000-0002-0000-0000-00000E000000}">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" prompt="Nama file ini bisa diketahui di folder dalam folder data bernama &quot;Point count data sheet original photos&quot;. Harus ditemukan foto data sheet ini sebelum di edit dan nama filenya ditulis disini." sqref="K1:K1048576">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" prompt="Nama file ini bisa diketahui di folder dalam folder data bernama &quot;Point count data sheet original photos&quot;. Harus ditemukan foto data sheet ini sebelum di edit dan nama filenya ditulis disini." sqref="K1:K1048576" xr:uid="{00000000-0002-0000-0000-00000F000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" prompt="Nama file ini bisa diketahui di folder dalam folder data bernama &quot;Point count data sheet EDITED photos&quot;. Harus ditemukan foto data sheet ini SETELAH di edit dan nama filenya ditulis disini." sqref="L1:L1048576">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" prompt="Nama file ini bisa diketahui di folder dalam folder data bernama &quot;Point count data sheet EDITED photos&quot;. Harus ditemukan foto data sheet ini SETELAH di edit dan nama filenya ditulis disini." sqref="L1:L1048576" xr:uid="{00000000-0002-0000-0000-000010000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="A = terdeteksi karena suaranya terdengar_x000d_V = terdeteksi karena terlihat_x000d_F = terdeteksi karena burungnya menerbang lewat titik tanpa mendarat." sqref="O1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="A = terdeteksi karena suaranya terdengar_x000d_V = terdeteksi karena terlihat_x000d_F = terdeteksi karena burungnya menerbang lewat titik tanpa mendarat." sqref="O1" xr:uid="{00000000-0002-0000-0000-000011000000}">
       <formula1>"A, V, F"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" prompt="Tulis nama orang yang mengedit data sheet ini. Cek dulu- orang yang mengedit data sheet ini harus adalah orang yg menulis data sheet ini." sqref="M1:M1048576">
+    <dataValidation type="textLength" showInputMessage="1" showErrorMessage="1" prompt="Tulis nama orang yang mengedit data sheet ini. Cek dulu- orang yang mengedit data sheet ini harus adalah orang yg menulis data sheet ini." sqref="M1:M1048576" xr:uid="{00000000-0002-0000-0000-000012000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Tulis nama orang yang memastikan bahwa data ini benar dan sama saja dengan data yg ditulis di data sheet asli." sqref="V1:V1048576"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Tulis nama orang yang memastikan bahwa data ini benar dan sama saja dengan data yg ditulis di data sheet asli." sqref="V1:V1048576" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="601" yWindow="221" count="1">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="Tulis nama spesies. Pakai nama latin dari buku burung Katie berjudul &quot;Birds of the Indonesian Archipelago&quot;">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" prompt="Tulis nama spesies. Pakai nama latin dari buku burung Katie berjudul &quot;Birds of the Indonesian Archipelago&quot;" xr:uid="{00000000-0002-0000-0000-000014000000}">
           <x14:formula1>
             <xm:f>'Species list'!$A$2:$A$445</xm:f>
           </x14:formula1>
@@ -2531,2236 +2529,2236 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A445"/>
   <sheetViews>
     <sheetView view="pageLayout" topLeftCell="A442" workbookViewId="0">
       <selection activeCell="A446" sqref="A446"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A118" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A119" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A121" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A122" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A123" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A124" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A133" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A134" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A135" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A136" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A137" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A138" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A139" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A143" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A144" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A145" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A146" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A147" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A148" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A149" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A150" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A151" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A152" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A153" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A154" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A155" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A156" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A157" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A158" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A159" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A160" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A161" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A162" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A163" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A164" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A165" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A166" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A167" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A168" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A169" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A170" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A171" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A172" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A173" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A174" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A175" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A176" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A177" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A178" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A179" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A180" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A181" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A182" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A183" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A184" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A185" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A186" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A187" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A188" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A189" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A190" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A191" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A192" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A193" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A194" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A195" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A196" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A197" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A198" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A199" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A200" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A201" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A202" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A203" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A204" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A205" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A206" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A207" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A208" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A209" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A210" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A211" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A212" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A213" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A214" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A215" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A216" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A217" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A218" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A219" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A220" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A221" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A222" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A223" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A224" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A225" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A226" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A227" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A228" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A229" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A230" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A231" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A232" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A233" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A234" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A235" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A236" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A237" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A238" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A239" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A240" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A241" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A242" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A243" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A244" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A245" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A246" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A247" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A248" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A249" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A250" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A251" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A252" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A253" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A254" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A255" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A256" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A257" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A258" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A259" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A260" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A261" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A262" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A263" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A264" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A265" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A266" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A267" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A268" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A269" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A270" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A271" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A272" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A273" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A274" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A275" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A276" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A277" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A278" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A279" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A280" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A281" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A282" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A283" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A284" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A285" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A286" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A287" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A288" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A289" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A290" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A291" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A292" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A293" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A294" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A295" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A296" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A297" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A298" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A299" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A300" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A301" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A302" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A303" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A304" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A305" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A306" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A307" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A308" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A309" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A310" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A311" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A312" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A313" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A314" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A315" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A316" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A317" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A318" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A319" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A320" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A321" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A322" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A323" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A324" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A325" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A326" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A327" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A328" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A329" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A330" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A331" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A332" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A333" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A334" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A335" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A336" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A337" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A338" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A339" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A340" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A341" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A342" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A343" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A344" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A345" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A346" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A347" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A348" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A349" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A350" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A351" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A352" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A353" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A354" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A355" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A356" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A357" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A358" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A359" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A360" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A361" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A362" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A363" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A364" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A365" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A366" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A367" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A368" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="369" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A369" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="370" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A370" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="371" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A371" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="372" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A372" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="373" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A373" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="374" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A374" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="375" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A375" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="376" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A376" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="377" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A377" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="378" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A378" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="379" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A379" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="380" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A380" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="381" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A381" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="382" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A382" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="383" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A383" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="384" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A384" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A385" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="386" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A386" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="387" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A387" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="388" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A388" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="389" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A389" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="390" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A390" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="391" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A391" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="392" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A392" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="393" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A393" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="394" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A394" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="395" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A395" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="396" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A396" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="397" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A397" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="398" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A398" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="399" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A399" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="400" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A400" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="401" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A401" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="402" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A402" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="403" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A403" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="404" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A404" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="405" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="405" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A405" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="406" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="406" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A406" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="407" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="407" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A407" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="408" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="408" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A408" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="409" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="409" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A409" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="410" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="410" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A410" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="411" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="411" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A411" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="412" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="412" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A412" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="413" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="413" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A413" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="414" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="414" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A414" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="415" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="415" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A415" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="416" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="416" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A416" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="417" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A417" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="418" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A418" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="419" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A419" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="420" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A420" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="421" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A421" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="422" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="422" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A422" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="423" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="423" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A423" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="424" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="424" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A424" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="425" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="425" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A425" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="426" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="426" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A426" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="427" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="427" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A427" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="428" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="428" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A428" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="429" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="429" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A429" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="430" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="430" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A430" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="431" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="431" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A431" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="432" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="432" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A432" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="433" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="433" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A433" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="434" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="434" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A434" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="435" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="435" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A435" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="436" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="436" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A436" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="437" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="437" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A437" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="438" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="438" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A438" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="439" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="439" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A439" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="440" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="440" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A440" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="441" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="441" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A441" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="442" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="442" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A442" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="443" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="443" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A443" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="444" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="444" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A444" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="445" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="445" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A445" t="s">
         <v>409</v>
       </c>

</xml_diff>